<commit_message>
Added the full inventory, still got prices to go, and whether or not they are on sale
</commit_message>
<xml_diff>
--- a/Broken Hill Surf Shop Inventory.xlsx
+++ b/Broken Hill Surf Shop Inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="100" windowWidth="28680" windowHeight="17460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="Inventory">Inventory!$A$1:$J$51</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,14 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Stock Code</t>
-  </si>
-  <si>
     <t>Supplier Code</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>Discounted Price</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>On Discount</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>Leashes</t>
   </si>
   <si>
-    <t>Scubber Gear</t>
-  </si>
-  <si>
     <t>Oxygen Tank</t>
   </si>
   <si>
@@ -112,12 +103,117 @@
   </si>
   <si>
     <t>Wet suit boot</t>
+  </si>
+  <si>
+    <t>Recreation</t>
+  </si>
+  <si>
+    <t>Beachball</t>
+  </si>
+  <si>
+    <t>Slippers</t>
+  </si>
+  <si>
+    <t>Water skis</t>
+  </si>
+  <si>
+    <t>Water recreation</t>
+  </si>
+  <si>
+    <t>Paddle board</t>
+  </si>
+  <si>
+    <t>Paddle stick</t>
+  </si>
+  <si>
+    <t>Oar</t>
+  </si>
+  <si>
+    <t>One man canoe</t>
+  </si>
+  <si>
+    <t>Two man canoe</t>
+  </si>
+  <si>
+    <t>Three man canoe</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>Rash shirt</t>
+  </si>
+  <si>
+    <t>Surf hat</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>Sunglasses</t>
+  </si>
+  <si>
+    <t>Sunscreen</t>
+  </si>
+  <si>
+    <t>Snorkeling Masks</t>
+  </si>
+  <si>
+    <t>Snorkeling Vest</t>
+  </si>
+  <si>
+    <t>Protection</t>
+  </si>
+  <si>
+    <t>First Aid Kit</t>
+  </si>
+  <si>
+    <t>Buoyancy Compensators</t>
+  </si>
+  <si>
+    <t>Regulator</t>
+  </si>
+  <si>
+    <t>Flashlight</t>
+  </si>
+  <si>
+    <t>Traction Pads</t>
+  </si>
+  <si>
+    <t>Surfboard Repair Kit</t>
+  </si>
+  <si>
+    <t>Board short</t>
+  </si>
+  <si>
+    <t>Swimming Trunks</t>
+  </si>
+  <si>
+    <t>Scuba Gear</t>
+  </si>
+  <si>
+    <t>Barcode Code</t>
+  </si>
+  <si>
+    <t>Beach towel</t>
+  </si>
+  <si>
+    <t>Esky</t>
+  </si>
+  <si>
+    <t>Life-Jacket</t>
+  </si>
+  <si>
+    <t>Board Bag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,7 +256,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -174,26 +270,83 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,15 +642,17 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="178" zoomScalePageLayoutView="178" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="19.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="7" width="8.83203125" style="2"/>
     <col min="8" max="9" width="16.83203125" customWidth="1"/>
     <col min="10" max="10" width="13.83203125" customWidth="1"/>
   </cols>
@@ -506,46 +661,52 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>5000100001</v>
+      <c r="B2" s="4">
+        <v>50010001</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>319</v>
+      </c>
+      <c r="G2" s="2">
+        <v>209</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -555,14 +716,20 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>5000200002</v>
+      <c r="B3" s="4">
+        <v>50020002</v>
       </c>
       <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
+      <c r="F3" s="2">
+        <v>419</v>
+      </c>
+      <c r="G3" s="2">
+        <v>309</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -572,43 +739,44 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>5000300003</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
+      <c r="B4" s="4">
+        <v>50030003</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="F4" s="3">
+        <v>449</v>
+      </c>
+      <c r="G4" s="3">
+        <v>329</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="1">
-        <v>1.5</v>
-      </c>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>5000400004</v>
+      <c r="B5" s="4">
+        <v>50040004</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="F5" s="2">
+        <v>169</v>
+      </c>
+      <c r="G5" s="2">
+        <v>129</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -618,14 +786,20 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>5000500005</v>
+      <c r="B6" s="4">
+        <v>50050005</v>
       </c>
       <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
+      <c r="G6" s="2">
+        <v>9</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -635,14 +809,20 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>5000600006</v>
+      <c r="B7" s="4">
+        <v>50060006</v>
       </c>
       <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
-        <v>18</v>
+      <c r="F7" s="2">
+        <v>1.29</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.89</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -652,14 +832,20 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>5000700007</v>
+      <c r="B8" s="4">
+        <v>50070007</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="F8" s="2">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2">
+        <v>15</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -669,14 +855,20 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>5000800008</v>
+      <c r="B9" s="4">
+        <v>50080008</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>51</v>
+      </c>
+      <c r="F9" s="2">
+        <v>22</v>
+      </c>
+      <c r="G9" s="2">
+        <v>15</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -686,14 +878,20 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>5000900009</v>
+      <c r="B10" s="4">
+        <v>50090009</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>52</v>
+      </c>
+      <c r="F10" s="2">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2">
+        <v>7</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -703,14 +901,20 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>5000100010</v>
+      <c r="B11" s="4">
+        <v>50100010</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>60</v>
+      </c>
+      <c r="F11" s="2">
+        <v>59</v>
+      </c>
+      <c r="G11" s="2">
+        <v>37</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -720,14 +924,20 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>5000110011</v>
+      <c r="B12" s="4">
+        <v>50110011</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="F12" s="2">
+        <v>80</v>
+      </c>
+      <c r="G12" s="2">
+        <v>50</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -737,14 +947,20 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>5000120012</v>
+      <c r="B13" s="4">
+        <v>50120012</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="F13" s="2">
+        <v>22</v>
+      </c>
+      <c r="G13" s="2">
+        <v>15</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -754,14 +970,20 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>5000130013</v>
+      <c r="B14" s="4">
+        <v>50130013</v>
       </c>
       <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" t="s">
-        <v>29</v>
+      <c r="F14" s="2">
+        <v>439</v>
+      </c>
+      <c r="G14" s="2">
+        <v>309</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -771,14 +993,20 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>5000140014</v>
+      <c r="B15" s="4">
+        <v>50140014</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
+      </c>
+      <c r="F15" s="2">
+        <v>22</v>
+      </c>
+      <c r="G15" s="2">
+        <v>17</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -788,14 +1016,20 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>5000150015</v>
+      <c r="B16" s="4">
+        <v>50150015</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="F16" s="2">
+        <v>33</v>
+      </c>
+      <c r="G16" s="2">
+        <v>25</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -805,14 +1039,20 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>5000160016</v>
+      <c r="B17" s="4">
+        <v>50160016</v>
       </c>
       <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="2">
+        <v>39</v>
+      </c>
+      <c r="G17" s="2">
         <v>25</v>
-      </c>
-      <c r="E17" t="s">
-        <v>22</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
@@ -822,14 +1062,20 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>5000170017</v>
+      <c r="B18" s="4">
+        <v>50170017</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="F18" s="2">
+        <v>29</v>
+      </c>
+      <c r="G18" s="2">
+        <v>14</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -839,14 +1085,20 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>5000180018</v>
+      <c r="B19" s="4">
+        <v>50180018</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="F19" s="2">
+        <v>23</v>
+      </c>
+      <c r="G19" s="2">
+        <v>16</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -856,14 +1108,20 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>5000190019</v>
+      <c r="B20" s="4">
+        <v>50190019</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>48</v>
+      </c>
+      <c r="F20" s="2">
+        <v>349</v>
+      </c>
+      <c r="G20" s="2">
+        <v>276</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -873,14 +1131,20 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>5000200020</v>
+      <c r="B21" s="4">
+        <v>50200020</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>49</v>
+      </c>
+      <c r="F21" s="2">
+        <v>249</v>
+      </c>
+      <c r="G21" s="2">
+        <v>165</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -890,11 +1154,20 @@
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22" s="4">
+        <v>50210021</v>
+      </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>50</v>
+      </c>
+      <c r="F22" s="2">
+        <v>59</v>
+      </c>
+      <c r="G22" s="2">
+        <v>43</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -904,11 +1177,14 @@
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" s="4">
+        <v>50220022</v>
+      </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -918,11 +1194,14 @@
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24" s="4">
+        <v>50230023</v>
+      </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H24" t="b">
         <v>0</v>
@@ -932,6 +1211,15 @@
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" s="4">
+        <v>50240024</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
       <c r="H25" t="b">
         <v>0</v>
       </c>
@@ -940,6 +1228,15 @@
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" s="4">
+        <v>50250025</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>24</v>
+      </c>
       <c r="H26" t="b">
         <v>0</v>
       </c>
@@ -948,6 +1245,15 @@
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" s="4">
+        <v>50260026</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
       <c r="H27" t="b">
         <v>0</v>
       </c>
@@ -956,6 +1262,15 @@
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" s="4">
+        <v>50270027</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
       <c r="H28" t="b">
         <v>0</v>
       </c>
@@ -964,6 +1279,15 @@
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" s="4">
+        <v>50280029</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
       <c r="H29" t="b">
         <v>0</v>
       </c>
@@ -972,6 +1296,15 @@
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" s="4">
+        <v>50290029</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
       <c r="H30" t="b">
         <v>0</v>
       </c>
@@ -980,6 +1313,15 @@
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" s="4">
+        <v>50300030</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
       <c r="H31" t="b">
         <v>0</v>
       </c>
@@ -988,6 +1330,15 @@
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="B32" s="4">
+        <v>50310031</v>
+      </c>
+      <c r="D32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
       <c r="H32" t="b">
         <v>0</v>
       </c>
@@ -996,6 +1347,15 @@
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="B33" s="4">
+        <v>50320032</v>
+      </c>
+      <c r="D33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
       <c r="H33" t="b">
         <v>0</v>
       </c>
@@ -1004,6 +1364,15 @@
       <c r="A34">
         <v>33</v>
       </c>
+      <c r="B34" s="4">
+        <v>50330033</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" t="s">
+        <v>29</v>
+      </c>
       <c r="H34" t="b">
         <v>0</v>
       </c>
@@ -1012,6 +1381,15 @@
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35" s="4">
+        <v>50340034</v>
+      </c>
+      <c r="D35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
       <c r="H35" t="b">
         <v>0</v>
       </c>
@@ -1020,6 +1398,15 @@
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="B36" s="4">
+        <v>50350035</v>
+      </c>
+      <c r="D36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" t="s">
+        <v>32</v>
+      </c>
       <c r="H36" t="b">
         <v>0</v>
       </c>
@@ -1028,6 +1415,15 @@
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="B37" s="4">
+        <v>50360036</v>
+      </c>
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
       <c r="H37" t="b">
         <v>0</v>
       </c>
@@ -1036,6 +1432,15 @@
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38" s="4">
+        <v>50370037</v>
+      </c>
+      <c r="D38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" t="s">
+        <v>35</v>
+      </c>
       <c r="H38" t="b">
         <v>0</v>
       </c>
@@ -1044,6 +1449,15 @@
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" s="4">
+        <v>50380038</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" t="s">
+        <v>36</v>
+      </c>
       <c r="H39" t="b">
         <v>0</v>
       </c>
@@ -1052,6 +1466,15 @@
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" s="4">
+        <v>50390039</v>
+      </c>
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" t="s">
+        <v>37</v>
+      </c>
       <c r="H40" t="b">
         <v>0</v>
       </c>
@@ -1060,6 +1483,15 @@
       <c r="A41">
         <v>40</v>
       </c>
+      <c r="B41" s="4">
+        <v>50400040</v>
+      </c>
+      <c r="D41" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" t="s">
+        <v>34</v>
+      </c>
       <c r="H41" t="b">
         <v>0</v>
       </c>
@@ -1068,6 +1500,15 @@
       <c r="A42">
         <v>41</v>
       </c>
+      <c r="B42" s="4">
+        <v>50410041</v>
+      </c>
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" t="s">
+        <v>59</v>
+      </c>
       <c r="H42" t="b">
         <v>0</v>
       </c>
@@ -1076,6 +1517,15 @@
       <c r="A43">
         <v>42</v>
       </c>
+      <c r="B43" s="4">
+        <v>50420042</v>
+      </c>
+      <c r="D43" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" t="s">
+        <v>39</v>
+      </c>
       <c r="H43" t="b">
         <v>0</v>
       </c>
@@ -1084,6 +1534,15 @@
       <c r="A44">
         <v>43</v>
       </c>
+      <c r="B44" s="4">
+        <v>50430043</v>
+      </c>
+      <c r="D44" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" t="s">
+        <v>53</v>
+      </c>
       <c r="H44" t="b">
         <v>0</v>
       </c>
@@ -1092,6 +1551,15 @@
       <c r="A45">
         <v>44</v>
       </c>
+      <c r="B45" s="4">
+        <v>50440044</v>
+      </c>
+      <c r="D45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" t="s">
+        <v>54</v>
+      </c>
       <c r="H45" t="b">
         <v>0</v>
       </c>
@@ -1100,6 +1568,15 @@
       <c r="A46">
         <v>45</v>
       </c>
+      <c r="B46" s="4">
+        <v>50450045</v>
+      </c>
+      <c r="D46" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" t="s">
+        <v>40</v>
+      </c>
       <c r="H46" t="b">
         <v>0</v>
       </c>
@@ -1108,6 +1585,15 @@
       <c r="A47">
         <v>46</v>
       </c>
+      <c r="B47" s="4">
+        <v>50460046</v>
+      </c>
+      <c r="D47" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" t="s">
+        <v>42</v>
+      </c>
       <c r="H47" t="b">
         <v>0</v>
       </c>
@@ -1116,6 +1602,15 @@
       <c r="A48">
         <v>47</v>
       </c>
+      <c r="B48" s="4">
+        <v>50470047</v>
+      </c>
+      <c r="D48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" t="s">
+        <v>57</v>
+      </c>
       <c r="H48" t="b">
         <v>0</v>
       </c>
@@ -1124,6 +1619,15 @@
       <c r="A49">
         <v>48</v>
       </c>
+      <c r="B49" s="4">
+        <v>50480048</v>
+      </c>
+      <c r="D49" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49" t="s">
+        <v>58</v>
+      </c>
       <c r="H49" t="b">
         <v>0</v>
       </c>
@@ -1132,6 +1636,15 @@
       <c r="A50">
         <v>49</v>
       </c>
+      <c r="B50" s="4">
+        <v>50490049</v>
+      </c>
+      <c r="D50" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" t="s">
+        <v>43</v>
+      </c>
       <c r="H50" t="b">
         <v>0</v>
       </c>
@@ -1139,6 +1652,15 @@
     <row r="51" spans="1:8">
       <c r="A51">
         <v>50</v>
+      </c>
+      <c r="B51" s="4">
+        <v>50500050</v>
+      </c>
+      <c r="D51" t="s">
+        <v>46</v>
+      </c>
+      <c r="E51" t="s">
+        <v>47</v>
       </c>
       <c r="H51" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added the full inventory, still got prices and discounts to go*
</commit_message>
<xml_diff>
--- a/Broken Hill Surf Shop Inventory.xlsx
+++ b/Broken Hill Surf Shop Inventory.xlsx
@@ -212,7 +212,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -302,8 +302,8 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -642,8 +642,8 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="178" zoomScalePageLayoutView="178" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1186,6 +1186,12 @@
       <c r="E23" t="s">
         <v>45</v>
       </c>
+      <c r="F23" s="2">
+        <v>60</v>
+      </c>
+      <c r="G23" s="2">
+        <v>40</v>
+      </c>
       <c r="H23" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
I added the sample barcode to github*
</commit_message>
<xml_diff>
--- a/Broken Hill Surf Shop Inventory.xlsx
+++ b/Broken Hill Surf Shop Inventory.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Discount Price</t>
   </si>
   <si>
-    <t>Surfboards</t>
-  </si>
-  <si>
     <t>Shortboards</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Bodyboards</t>
   </si>
   <si>
-    <t>Surfboard Accessories</t>
-  </si>
-  <si>
     <t>Fins</t>
   </si>
   <si>
@@ -208,6 +202,9 @@
   </si>
   <si>
     <t>Swimming Goggles</t>
+  </si>
+  <si>
+    <t>Surfing</t>
   </si>
 </sst>
 </file>
@@ -645,8 +642,8 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="178" zoomScalePageLayoutView="178" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -665,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -700,10 +697,10 @@
         <v>50010001</v>
       </c>
       <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="2">
         <v>319</v>
@@ -723,10 +720,10 @@
         <v>50020002</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2">
         <v>419</v>
@@ -746,10 +743,10 @@
         <v>50030003</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3">
         <v>449</v>
@@ -770,10 +767,10 @@
         <v>50040004</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2">
         <v>169</v>
@@ -793,10 +790,10 @@
         <v>50050005</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2">
         <v>16</v>
@@ -816,10 +813,10 @@
         <v>50060006</v>
       </c>
       <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
       </c>
       <c r="F7" s="2">
         <v>1.29</v>
@@ -839,10 +836,10 @@
         <v>50070007</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2">
         <v>24</v>
@@ -862,10 +859,10 @@
         <v>50080008</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F9" s="2">
         <v>22</v>
@@ -885,10 +882,10 @@
         <v>50090009</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F10" s="2">
         <v>17</v>
@@ -908,10 +905,10 @@
         <v>50100010</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F11" s="2">
         <v>59</v>
@@ -931,10 +928,10 @@
         <v>50110011</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F12" s="2">
         <v>80</v>
@@ -954,10 +951,10 @@
         <v>50120012</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" s="2">
         <v>22</v>
@@ -977,10 +974,10 @@
         <v>50130013</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F14" s="2">
         <v>439</v>
@@ -1000,10 +997,10 @@
         <v>50140014</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2">
         <v>22</v>
@@ -1023,10 +1020,10 @@
         <v>50150015</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F16" s="2">
         <v>33</v>
@@ -1046,10 +1043,10 @@
         <v>50160016</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F17" s="2">
         <v>39</v>
@@ -1069,10 +1066,10 @@
         <v>50170017</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F18" s="2">
         <v>29</v>
@@ -1092,10 +1089,10 @@
         <v>50180018</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F19" s="2">
         <v>23</v>
@@ -1115,10 +1112,10 @@
         <v>50190019</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F20" s="2">
         <v>349</v>
@@ -1138,10 +1135,10 @@
         <v>50200020</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F21" s="2">
         <v>249</v>
@@ -1161,10 +1158,10 @@
         <v>50210021</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F22" s="2">
         <v>59</v>
@@ -1184,10 +1181,10 @@
         <v>50220022</v>
       </c>
       <c r="D23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F23" s="2">
         <v>60</v>
@@ -1207,10 +1204,10 @@
         <v>50230023</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F24" s="2">
         <v>14</v>
@@ -1230,10 +1227,10 @@
         <v>50240024</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F25" s="2">
         <v>439</v>
@@ -1253,10 +1250,10 @@
         <v>50250025</v>
       </c>
       <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" t="s">
         <v>22</v>
-      </c>
-      <c r="E26" t="s">
-        <v>24</v>
       </c>
       <c r="F26" s="2">
         <v>22</v>
@@ -1276,10 +1273,10 @@
         <v>50260026</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F27" s="2">
         <v>33</v>
@@ -1299,10 +1296,10 @@
         <v>50270027</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F28" s="2">
         <v>39</v>
@@ -1322,10 +1319,10 @@
         <v>50280029</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F29" s="2">
         <v>29</v>
@@ -1345,10 +1342,10 @@
         <v>50290029</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F30" s="2">
         <v>23</v>
@@ -1368,10 +1365,10 @@
         <v>50300030</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
@@ -1385,10 +1382,10 @@
         <v>50310031</v>
       </c>
       <c r="D32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H32" t="b">
         <v>0</v>
@@ -1402,10 +1399,10 @@
         <v>50320032</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -1419,10 +1416,10 @@
         <v>50330033</v>
       </c>
       <c r="D34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" t="s">
         <v>27</v>
-      </c>
-      <c r="E34" t="s">
-        <v>29</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
@@ -1436,10 +1433,10 @@
         <v>50340034</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E35" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -1453,10 +1450,10 @@
         <v>50350035</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H36" t="b">
         <v>0</v>
@@ -1470,10 +1467,10 @@
         <v>50360036</v>
       </c>
       <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
         <v>31</v>
-      </c>
-      <c r="E37" t="s">
-        <v>33</v>
       </c>
       <c r="H37" t="b">
         <v>0</v>
@@ -1487,10 +1484,10 @@
         <v>50370037</v>
       </c>
       <c r="D38" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
@@ -1504,10 +1501,10 @@
         <v>50380038</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H39" t="b">
         <v>0</v>
@@ -1521,10 +1518,10 @@
         <v>50390039</v>
       </c>
       <c r="D40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H40" t="b">
         <v>0</v>
@@ -1538,10 +1535,10 @@
         <v>50400040</v>
       </c>
       <c r="D41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H41" t="b">
         <v>0</v>
@@ -1555,10 +1552,10 @@
         <v>50410041</v>
       </c>
       <c r="D42" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H42" t="b">
         <v>0</v>
@@ -1572,10 +1569,10 @@
         <v>50420042</v>
       </c>
       <c r="D43" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H43" t="b">
         <v>0</v>
@@ -1589,10 +1586,10 @@
         <v>50430043</v>
       </c>
       <c r="D44" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H44" t="b">
         <v>0</v>
@@ -1606,10 +1603,10 @@
         <v>50440044</v>
       </c>
       <c r="D45" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H45" t="b">
         <v>0</v>
@@ -1623,10 +1620,10 @@
         <v>50450045</v>
       </c>
       <c r="D46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H46" t="b">
         <v>0</v>
@@ -1640,10 +1637,10 @@
         <v>50460046</v>
       </c>
       <c r="D47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H47" t="b">
         <v>0</v>
@@ -1657,10 +1654,10 @@
         <v>50470047</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E48" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H48" t="b">
         <v>0</v>
@@ -1674,10 +1671,10 @@
         <v>50480048</v>
       </c>
       <c r="D49" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E49" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H49" t="b">
         <v>0</v>
@@ -1691,10 +1688,10 @@
         <v>50490049</v>
       </c>
       <c r="D50" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H50" t="b">
         <v>0</v>
@@ -1708,10 +1705,10 @@
         <v>50500050</v>
       </c>
       <c r="D51" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E51" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H51" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Finished the product database, and i also put in separate sheets that show customer and supplier details. Not gonna do anymore work this weekend, cos of Band Camp packing and preparing*
</commit_message>
<xml_diff>
--- a/Broken Hill Surf Shop Inventory.xlsx
+++ b/Broken Hill Surf Shop Inventory.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
+    <sheet name="Suppliers" sheetId="2" r:id="rId2"/>
+    <sheet name="Customer" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Inventory">Inventory!$A$1:$J$51</definedName>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -48,9 +50,6 @@
     <t>On Discount</t>
   </si>
   <si>
-    <t>Discount Price</t>
-  </si>
-  <si>
     <t>Shortboards</t>
   </si>
   <si>
@@ -205,6 +204,120 @@
   </si>
   <si>
     <t>Surfing</t>
+  </si>
+  <si>
+    <t>Discount Value</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ABN (Australian Business Number)/International Company Identifier)</t>
+  </si>
+  <si>
+    <t>ABN 13718749829</t>
+  </si>
+  <si>
+    <t>ABN 22398752957</t>
+  </si>
+  <si>
+    <t>ABN 70823929385</t>
+  </si>
+  <si>
+    <t>ABN 52423985420</t>
+  </si>
+  <si>
+    <t>CXXYF67251</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>76 Toshuo Street, Shanghai 200000, China</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Dylan</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Oo</t>
+  </si>
+  <si>
+    <t>Georgy</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Jimmy</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>10 Smith Street, Jimville 2341,  Sydney, Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">178 Wave Street, Alextown 2987, Sydney, Australia </t>
+  </si>
+  <si>
+    <t>154 Sandy Road, Hope 2198, Sydney, Australia</t>
+  </si>
+  <si>
+    <t>34 Coral Crescent, Stanwell Valley 2876 Sydney, Australia</t>
+  </si>
+  <si>
+    <t>17 Assassin Road, Frank 6123, Fremantle, Australia</t>
+  </si>
+  <si>
+    <t>13 Gaga Road, Illawong 2234, Sydney, Australia</t>
+  </si>
+  <si>
+    <t>87 Funny Road, Alexandria 2483, Sydney, Australia</t>
+  </si>
+  <si>
+    <t>321 Hots Road, Padstow 2149, Sydney, Australia</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Zhang</t>
+  </si>
+  <si>
+    <t>763 Quazho Road, Beijing 100000, China</t>
   </si>
 </sst>
 </file>
@@ -256,8 +369,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -299,16 +426,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -328,6 +453,13 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -347,6 +479,13 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -641,28 +780,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="178" zoomScalePageLayoutView="178" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="B1" zoomScale="178" zoomScaleNormal="178" zoomScalePageLayoutView="178" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="16.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="19.1640625" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="7" width="8.83203125" style="2"/>
-    <col min="8" max="9" width="16.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="6" max="7" width="8.83203125" style="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12" style="4" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>54</v>
+      <c r="B1" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -673,19 +813,19 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="I1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -693,19 +833,22 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>50010001</v>
       </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
         <v>319</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>209</v>
       </c>
       <c r="H2" t="b">
@@ -716,19 +859,22 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>50020002</v>
       </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1">
         <v>419</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>309</v>
       </c>
       <c r="H3" t="b">
@@ -739,43 +885,55 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>50030003</v>
       </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3">
-        <v>449</v>
-      </c>
-      <c r="G4" s="3">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
+        <v>450</v>
+      </c>
+      <c r="G4" s="2">
         <v>329</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="I4" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="2">
+        <f>F4 - (F4 * I4)</f>
+        <v>405</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>50040004</v>
       </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1">
         <v>169</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>129</v>
       </c>
       <c r="H5" t="b">
@@ -786,19 +944,22 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>50050005</v>
       </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1">
         <v>16</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>9</v>
       </c>
       <c r="H6" t="b">
@@ -809,19 +970,22 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>50060006</v>
       </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="2">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1">
         <v>1.29</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>0.89</v>
       </c>
       <c r="H7" t="b">
@@ -832,19 +996,22 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>50070007</v>
       </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="2">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1">
         <v>24</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>15</v>
       </c>
       <c r="H8" t="b">
@@ -855,19 +1022,22 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>50080008</v>
       </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="2">
+        <v>48</v>
+      </c>
+      <c r="F9" s="1">
         <v>22</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>15</v>
       </c>
       <c r="H9" t="b">
@@ -878,19 +1048,22 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>50090009</v>
       </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="2">
+        <v>49</v>
+      </c>
+      <c r="F10" s="1">
         <v>17</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>7</v>
       </c>
       <c r="H10" t="b">
@@ -901,19 +1074,22 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>50100010</v>
       </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="2">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1">
         <v>59</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>37</v>
       </c>
       <c r="H11" t="b">
@@ -924,42 +1100,55 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>50110011</v>
       </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="2">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1">
         <v>80</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>50</v>
       </c>
       <c r="H12" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J12" s="1">
+        <f>F12-(F12*I12)</f>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>50120012</v>
       </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="2">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1">
         <v>22</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>15</v>
       </c>
       <c r="H13" t="b">
@@ -970,19 +1159,22 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>50130013</v>
       </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="2">
+        <v>17</v>
+      </c>
+      <c r="F14" s="1">
         <v>439</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>309</v>
       </c>
       <c r="H14" t="b">
@@ -993,19 +1185,22 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>50140014</v>
       </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="1">
         <v>22</v>
       </c>
-      <c r="F15" s="2">
-        <v>22</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>17</v>
       </c>
       <c r="H15" t="b">
@@ -1016,654 +1211,890 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>50150015</v>
       </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="2">
+        <v>22</v>
+      </c>
+      <c r="F16" s="1">
         <v>33</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>25</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>50160016</v>
       </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="2">
+        <v>23</v>
+      </c>
+      <c r="F17" s="1">
         <v>39</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>25</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>50170017</v>
       </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="2">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1">
         <v>29</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>14</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>50180018</v>
       </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="2">
+        <v>20</v>
+      </c>
+      <c r="F19" s="1">
         <v>23</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <v>16</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>50190019</v>
       </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="2">
-        <v>349</v>
-      </c>
-      <c r="G20" s="2">
+        <v>45</v>
+      </c>
+      <c r="F20" s="1">
+        <v>350</v>
+      </c>
+      <c r="G20" s="1">
         <v>276</v>
       </c>
       <c r="H20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J20" s="1">
+        <f>F20-(F20*I20)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>50200020</v>
       </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="2">
+        <v>46</v>
+      </c>
+      <c r="F21" s="1">
         <v>249</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>165</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>50210021</v>
       </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="2">
+        <v>47</v>
+      </c>
+      <c r="F22" s="1">
         <v>59</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
         <v>43</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>50220022</v>
       </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="2">
+        <v>42</v>
+      </c>
+      <c r="F23" s="1">
         <v>60</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <v>40</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>50230023</v>
       </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" s="2">
+        <v>58</v>
+      </c>
+      <c r="F24" s="1">
         <v>14</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <v>8</v>
       </c>
       <c r="H24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>50240024</v>
       </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="2">
+        <v>17</v>
+      </c>
+      <c r="F25" s="1">
         <v>439</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <v>309</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>50250025</v>
       </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="1">
         <v>22</v>
       </c>
-      <c r="F26" s="2">
-        <v>22</v>
-      </c>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
         <v>17</v>
       </c>
       <c r="H26" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>50260026</v>
       </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="2">
+        <v>22</v>
+      </c>
+      <c r="F27" s="1">
         <v>33</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="1">
         <v>25</v>
       </c>
       <c r="H27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="J27" s="1">
+        <f>F27-(F27*I27)</f>
+        <v>24.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>50270027</v>
       </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="2">
+        <v>23</v>
+      </c>
+      <c r="F28" s="1">
         <v>39</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
         <v>25</v>
       </c>
       <c r="H28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>50280029</v>
       </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="2">
+        <v>18</v>
+      </c>
+      <c r="F29" s="1">
         <v>29</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
         <v>14</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>50290029</v>
       </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" s="2">
+        <v>41</v>
+      </c>
+      <c r="F30" s="1">
         <v>23</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
         <v>16</v>
       </c>
       <c r="H30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>50300030</v>
       </c>
+      <c r="C31" t="s">
+        <v>62</v>
+      </c>
       <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="1">
         <v>20</v>
       </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="2">
-        <v>20</v>
-      </c>
-      <c r="G31" s="2">
+      <c r="G31" s="1">
         <v>14</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>50310031</v>
       </c>
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="F32" s="1">
+        <v>49</v>
+      </c>
+      <c r="G32" s="1">
+        <v>30</v>
       </c>
       <c r="H32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>50320032</v>
       </c>
+      <c r="C33" t="s">
+        <v>63</v>
+      </c>
       <c r="D33" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" t="s">
         <v>25</v>
       </c>
-      <c r="E33" t="s">
-        <v>26</v>
+      <c r="F33" s="1">
+        <v>9</v>
+      </c>
+      <c r="G33" s="1">
+        <v>5</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="3">
         <v>50330033</v>
       </c>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="F34" s="1">
+        <v>5</v>
+      </c>
+      <c r="G34" s="1">
+        <v>3</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>50340034</v>
       </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="F35" s="1">
+        <v>299</v>
+      </c>
+      <c r="G35" s="1">
+        <v>159</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="3">
         <v>50350035</v>
       </c>
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
       <c r="D36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
         <v>29</v>
       </c>
-      <c r="E36" t="s">
-        <v>30</v>
+      <c r="F36" s="1">
+        <v>699</v>
+      </c>
+      <c r="G36" s="1">
+        <v>415</v>
       </c>
       <c r="H36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>50360036</v>
       </c>
+      <c r="C37" t="s">
+        <v>63</v>
+      </c>
       <c r="D37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E37" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="F37" s="1">
+        <v>99</v>
+      </c>
+      <c r="G37" s="1">
+        <v>49</v>
       </c>
       <c r="H37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>50370037</v>
       </c>
+      <c r="C38" t="s">
+        <v>63</v>
+      </c>
       <c r="D38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E38" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F38" s="1">
+        <v>329</v>
+      </c>
+      <c r="G38" s="1">
+        <v>219</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>50380038</v>
       </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
       <c r="D39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E39" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="F39" s="1">
+        <v>450</v>
+      </c>
+      <c r="G39" s="1">
+        <v>319</v>
       </c>
       <c r="H39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J39" s="1">
+        <f>F39-(F39*I39)</f>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>50390039</v>
       </c>
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
       <c r="D40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="F40" s="1">
+        <v>599</v>
+      </c>
+      <c r="G40" s="1">
+        <v>359</v>
       </c>
       <c r="H40" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>50400040</v>
       </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
       <c r="D41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E41" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="F41" s="1">
+        <v>19</v>
+      </c>
+      <c r="G41" s="1">
+        <v>13</v>
       </c>
       <c r="H41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="3">
         <v>50410041</v>
       </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
       <c r="D42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E42" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="F42" s="1">
+        <v>63</v>
+      </c>
+      <c r="G42" s="1">
+        <v>34</v>
       </c>
       <c r="H42" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="3">
         <v>50420042</v>
       </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
       <c r="D43" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" t="s">
         <v>36</v>
       </c>
-      <c r="E43" t="s">
-        <v>37</v>
+      <c r="F43" s="1">
+        <v>29</v>
+      </c>
+      <c r="G43" s="1">
+        <v>19</v>
       </c>
       <c r="H43" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="3">
         <v>50430043</v>
       </c>
+      <c r="C44" t="s">
+        <v>64</v>
+      </c>
       <c r="D44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E44" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="F44" s="1">
+        <v>89</v>
+      </c>
+      <c r="G44" s="1">
+        <v>45</v>
       </c>
       <c r="H44" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="3">
         <v>50440044</v>
       </c>
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
       <c r="D45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E45" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="F45" s="1">
+        <v>20</v>
+      </c>
+      <c r="G45" s="1">
+        <v>14</v>
       </c>
       <c r="H45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J45" s="1">
+        <f>F45-(F45*I45)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="3">
         <v>50450045</v>
       </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
       <c r="D46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E46" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="F46" s="1">
+        <v>29</v>
+      </c>
+      <c r="G46" s="1">
+        <v>15</v>
       </c>
       <c r="H46" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" s="3">
         <v>50460046</v>
       </c>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
       <c r="D47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" t="s">
         <v>39</v>
       </c>
-      <c r="E47" t="s">
-        <v>40</v>
+      <c r="F47" s="1">
+        <v>150</v>
+      </c>
+      <c r="G47" s="1">
+        <v>69</v>
       </c>
       <c r="H47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="J47" s="1">
+        <f>F47-(F47*I47)</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48" s="3">
         <v>50470047</v>
       </c>
+      <c r="C48" t="s">
+        <v>65</v>
+      </c>
       <c r="D48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E48" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="F48" s="1">
+        <v>29</v>
+      </c>
+      <c r="G48" s="1">
+        <v>15</v>
       </c>
       <c r="H48" t="b">
         <v>0</v>
@@ -1673,14 +2104,23 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="3">
         <v>50480048</v>
       </c>
+      <c r="C49" t="s">
+        <v>65</v>
+      </c>
       <c r="D49" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" t="s">
+        <v>55</v>
+      </c>
+      <c r="F49" s="1">
+        <v>60</v>
+      </c>
+      <c r="G49" s="1">
         <v>39</v>
-      </c>
-      <c r="E49" t="s">
-        <v>56</v>
       </c>
       <c r="H49" t="b">
         <v>0</v>
@@ -1690,14 +2130,23 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="3">
         <v>50490049</v>
       </c>
+      <c r="C50" t="s">
+        <v>65</v>
+      </c>
       <c r="D50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E50" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="F50" s="1">
+        <v>25</v>
+      </c>
+      <c r="G50" s="1">
+        <v>16</v>
       </c>
       <c r="H50" t="b">
         <v>0</v>
@@ -1707,14 +2156,23 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="3">
         <v>50500050</v>
       </c>
+      <c r="C51" t="s">
+        <v>65</v>
+      </c>
       <c r="D51" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" t="s">
         <v>44</v>
       </c>
-      <c r="E51" t="s">
-        <v>45</v>
+      <c r="F51" s="1">
+        <v>89</v>
+      </c>
+      <c r="G51" s="1">
+        <v>46</v>
       </c>
       <c r="H51" t="b">
         <v>0</v>
@@ -1729,4 +2187,248 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView zoomScale="178" zoomScaleNormal="178" zoomScalePageLayoutView="178" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="52.1640625" customWidth="1"/>
+    <col min="5" max="5" width="43.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="178" zoomScalePageLayoutView="178" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="42.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="3">
+        <v>91241233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="3">
+        <v>91323891</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="3">
+        <v>92387644</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="3">
+        <v>93927522</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="3">
+        <v>91294791</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>